<commit_message>
EQWin fetch now works
</commit_message>
<xml_diff>
--- a/data/WRBdata.xlsx
+++ b/data/WRBdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g_del\Documents\R\YG work\Packages\WRBTrends\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2424B8A-D42F-4E9E-A53D-559F05CB381F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55071EBA-A1D8-4800-86E8-48F5E6C24BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2532" yWindow="2532" windowWidth="17280" windowHeight="9984" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="11" r:id="rId1"/>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="465">
   <si>
     <t>Note for Ellorie: This is a work in progress, but reflects how I'm trying to work with this metadata workbook in R.  It's intended for us a bit, but more so that someone else can reproduce what we're doing here in future years without trouble.</t>
   </si>
@@ -1552,6 +1552,12 @@
   </si>
   <si>
     <t>Water Temp</t>
+  </si>
+  <si>
+    <t>pH-F</t>
+  </si>
+  <si>
+    <t>EQWin</t>
   </si>
 </sst>
 </file>
@@ -2032,13 +2038,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A2:T167"/>
+  <dimension ref="A2:T169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B147" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="C171" sqref="C171:E175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6145,13 +6151,13 @@
         <v>254</v>
       </c>
       <c r="B165" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C165" t="s">
-        <v>129</v>
+        <v>463</v>
       </c>
       <c r="D165" t="s">
-        <v>30</v>
+        <v>464</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6162,7 +6168,7 @@
         <v>255</v>
       </c>
       <c r="C166" t="s">
-        <v>462</v>
+        <v>129</v>
       </c>
       <c r="D166" t="s">
         <v>30</v>
@@ -6176,10 +6182,38 @@
         <v>255</v>
       </c>
       <c r="C167" t="s">
+        <v>462</v>
+      </c>
+      <c r="D167" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A168" t="s">
+        <v>254</v>
+      </c>
+      <c r="B168" t="s">
+        <v>255</v>
+      </c>
+      <c r="C168" t="s">
         <v>133</v>
       </c>
-      <c r="D167" t="s">
-        <v>30</v>
+      <c r="D168" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A169" t="s">
+        <v>254</v>
+      </c>
+      <c r="B169" t="s">
+        <v>255</v>
+      </c>
+      <c r="C169" t="s">
+        <v>463</v>
+      </c>
+      <c r="D169" t="s">
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -11419,15 +11453,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <URL xmlns="http://schemas.microsoft.com/sharepoint/v3">
@@ -11444,7 +11469,62 @@
 </p:properties>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Link to a Document" ma:contentTypeID="0x01010A00C00CEA10C005BB4DA0CFB44DA0ECE6B1" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a link to a document in a different location." ma:contentTypeScope="" ma:versionID="e3f3326e9f05b7a04e6a82246aaa09b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="735eeb13-47b0-4f7e-9a38-605dfa23e887" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5a06d2b95cf9ebd97a30b99af6286c54" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -11618,61 +11698,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=14.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5A74EB8-8E1C-4D86-B9DA-6A928EB71FF2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDB4E8F1-A738-4EA3-B570-EDAE7229C042}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11684,7 +11710,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5A74EB8-8E1C-4D86-B9DA-6A928EB71FF2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D9AF136-3CF9-47F0-B0DE-4EC61FC78DCC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C12822C-7DB8-432E-A7D8-9419849450F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11702,12 +11744,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D9AF136-3CF9-47F0-B0DE-4EC61FC78DCC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>